<commit_message>
Edit the total protein concdentration files (all have 3 columns)
</commit_message>
<xml_diff>
--- a/inst/dataInst/R023_Mel133_sample_conc_EZQ.xlsx
+++ b/inst/dataInst/R023_Mel133_sample_conc_EZQ.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3620" yWindow="60" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="3740" yWindow="0" windowWidth="25120" windowHeight="15580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="adjusted results" sheetId="4" r:id="rId1"/>
@@ -489,8 +489,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="161">
+  <cellStyleXfs count="167">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -667,7 +673,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="161">
+  <cellStyles count="167">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -748,6 +754,9 @@
     <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -828,6 +837,9 @@
     <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1159,8 +1171,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C66"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>